<commit_message>
Fixed suppression map bug.
</commit_message>
<xml_diff>
--- a/Supporting R Code/WindEquations Nelson2002.xlsx
+++ b/Supporting R Code/WindEquations Nelson2002.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Wind equations from Nelson 2002</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>EffectiveWindSpeed</t>
-  </si>
-  <si>
-    <t>Equation 6</t>
   </si>
 </sst>
 </file>
@@ -399,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,12 +411,12 @@
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -438,11 +435,8 @@
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -461,24 +455,21 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>18</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D6">
         <f>+E6-F6</f>
@@ -490,18 +481,19 @@
       <c r="F6">
         <v>24</v>
       </c>
-      <c r="I6">
-        <f>+SIN(C6^2)</f>
-        <v>-0.49102159389846933</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B9">
-        <f>+B6*(((A6/B6)^2+2*(A6/B6)*SIN(C6)*COS(D6)+SIN(C6^2))^0.5)</f>
-        <v>13.799401158440215</v>
+        <f>+B6*(((A6/B6)^2+2*(A6/B6)*SIN(C6)*COS(D6)+SIN(C6)^2)^0.5)</f>
+        <v>33.316263441614133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes to effective wind speed (tricky!).
</commit_message>
<xml_diff>
--- a/Supporting R Code/WindEquations Nelson2002.xlsx
+++ b/Supporting R Code/WindEquations Nelson2002.xlsx
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,272 +487,241 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <f>+E9-F9</f>
-        <v>360</v>
-      </c>
-      <c r="E9">
-        <v>360</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f>+B9*(((A9/B9)^2+2*(A9/B9)*SIN(C9/180*PI())*COS(D9/180*PI())+(SIN(C9/180*PI())^2))^0.5)</f>
-        <v>6.2940952255126037</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10:D17" si="0">+E10-F10</f>
+        <f>+E10-F10</f>
+        <v>140</v>
+      </c>
+      <c r="E10">
+        <v>140</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>+B10*(((A10/B10)^2+2*(A10/B10)*SIN(C10/180*PI())*COS(D10/180*PI())+(SIN(C10/180*PI())^2))^0.5)</f>
+        <v>7.6712899367660032</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <f>+E12-F12</f>
+        <v>360</v>
+      </c>
+      <c r="E12">
+        <v>360</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f>+B12*(((A12/B12)^2+2*(A12/B12)*SIN(C12/180*PI())*COS(D12/180*PI())+(SIN(C12/180*PI())^2))^0.5)</f>
+        <v>6.2940952255126037</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D20" si="0">+E13-F13</f>
         <v>315</v>
       </c>
-      <c r="E10">
-        <v>360</v>
-      </c>
-      <c r="F10">
+      <c r="E13">
+        <v>360</v>
+      </c>
+      <c r="F13">
         <v>45</v>
       </c>
-      <c r="H10">
-        <f t="shared" ref="H10:H17" si="1">+B10*(((A10/B10)^2+2*(A10/B10)*SIN(C10/180*PI())*COS(D10/180*PI())+(SIN(C10/180*PI())^2))^0.5)</f>
+      <c r="H13">
+        <f t="shared" ref="H13:H20" si="1">+B13*(((A13/B13)^2+2*(A13/B13)*SIN(C13/180*PI())*COS(D13/180*PI())+(SIN(C13/180*PI())^2))^0.5)</f>
         <v>5.9854254274283196</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>15</v>
-      </c>
-      <c r="D11">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>270</v>
       </c>
-      <c r="E11">
-        <v>360</v>
-      </c>
-      <c r="F11">
+      <c r="E14">
+        <v>360</v>
+      </c>
+      <c r="F14">
         <v>90</v>
       </c>
-      <c r="H11">
+      <c r="H14">
         <f t="shared" si="1"/>
         <v>5.1647538617725539</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>15</v>
-      </c>
-      <c r="D12">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
-      <c r="E12">
-        <v>360</v>
-      </c>
-      <c r="F12">
+      <c r="E15">
+        <v>360</v>
+      </c>
+      <c r="F15">
         <v>135</v>
       </c>
-      <c r="H12">
+      <c r="H15">
         <f t="shared" si="1"/>
         <v>4.1861733549966074</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>15</v>
-      </c>
-      <c r="D13">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="E13">
-        <v>360</v>
-      </c>
-      <c r="F13">
-        <v>180</v>
-      </c>
-      <c r="H13">
+      <c r="E16">
+        <v>360</v>
+      </c>
+      <c r="F16">
+        <v>180</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="1"/>
         <v>3.7059047744873963</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>15</v>
-      </c>
-      <c r="D14">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
-      <c r="E14">
-        <v>360</v>
-      </c>
-      <c r="F14">
+      <c r="E17">
+        <v>360</v>
+      </c>
+      <c r="F17">
         <v>225</v>
       </c>
-      <c r="H14">
+      <c r="H17">
         <f t="shared" si="1"/>
         <v>4.1861733549966074</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>15</v>
-      </c>
-      <c r="D15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="E15">
-        <v>360</v>
-      </c>
-      <c r="F15">
+      <c r="E18">
+        <v>360</v>
+      </c>
+      <c r="F18">
         <v>270</v>
       </c>
-      <c r="H15">
+      <c r="H18">
         <f t="shared" si="1"/>
         <v>5.1647538617725539</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>15</v>
-      </c>
-      <c r="D16">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E16">
-        <v>360</v>
-      </c>
-      <c r="F16">
+      <c r="E19">
+        <v>360</v>
+      </c>
+      <c r="F19">
         <v>315</v>
       </c>
-      <c r="H16">
+      <c r="H19">
         <f t="shared" si="1"/>
         <v>5.9854254274283196</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>15</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>360</v>
-      </c>
-      <c r="F17">
-        <v>360</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
-        <v>6.2940952255126037</v>
-      </c>
-      <c r="J17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19">
-        <v>15</v>
-      </c>
-      <c r="D19">
-        <f>+E19-F19</f>
-        <v>360</v>
-      </c>
-      <c r="E19">
-        <v>360</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <f>+B19*(((A19/B19)^2+2*(A19/B19)*SIN(C19/180*PI())*COS(D19/180*PI())+(SIN(C19/180*PI())^2))^0.5)</f>
-        <v>7.5881904510252074</v>
-      </c>
-      <c r="J19" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -760,537 +729,509 @@
         <v>5</v>
       </c>
       <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>360</v>
+      </c>
+      <c r="F20">
+        <v>360</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>6.2940952255126037</v>
+      </c>
+      <c r="J20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
         <v>10</v>
       </c>
-      <c r="C20">
-        <v>15</v>
-      </c>
-      <c r="D20">
-        <f t="shared" ref="D20:D27" si="2">+E20-F20</f>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <f>+E22-F22</f>
+        <v>360</v>
+      </c>
+      <c r="E22">
+        <v>360</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>+B22*(((A22/B22)^2+2*(A22/B22)*SIN(C22/180*PI())*COS(D22/180*PI())+(SIN(C22/180*PI())^2))^0.5)</f>
+        <v>7.5881904510252074</v>
+      </c>
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:D30" si="2">+E23-F23</f>
         <v>315</v>
       </c>
-      <c r="E20">
-        <v>360</v>
-      </c>
-      <c r="F20">
+      <c r="E23">
+        <v>360</v>
+      </c>
+      <c r="F23">
         <v>45</v>
       </c>
-      <c r="H20">
-        <f t="shared" ref="H20:H27" si="3">+B20*(((A20/B20)^2+2*(A20/B20)*SIN(C20/180*PI())*COS(D20/180*PI())+(SIN(C20/180*PI())^2))^0.5)</f>
+      <c r="H23">
+        <f t="shared" ref="H23:H30" si="3">+B23*(((A23/B23)^2+2*(A23/B23)*SIN(C23/180*PI())*COS(D23/180*PI())+(SIN(C23/180*PI())^2))^0.5)</f>
         <v>7.0710678118654746</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
         <v>10</v>
       </c>
-      <c r="C21">
-        <v>15</v>
-      </c>
-      <c r="D21">
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-      <c r="E21">
-        <v>360</v>
-      </c>
-      <c r="F21">
+      <c r="E24">
+        <v>360</v>
+      </c>
+      <c r="F24">
         <v>90</v>
       </c>
-      <c r="H21">
+      <c r="H24">
         <f t="shared" si="3"/>
         <v>5.6301625030524702</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>5</v>
-      </c>
-      <c r="B22">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
         <v>10</v>
       </c>
-      <c r="C22">
-        <v>15</v>
-      </c>
-      <c r="D22">
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="2"/>
         <v>225</v>
       </c>
-      <c r="E22">
-        <v>360</v>
-      </c>
-      <c r="F22">
+      <c r="E25">
+        <v>360</v>
+      </c>
+      <c r="F25">
         <v>135</v>
       </c>
-      <c r="H22">
+      <c r="H25">
         <f t="shared" si="3"/>
         <v>3.6602540378443855</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>5</v>
-      </c>
-      <c r="B23">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
         <v>10</v>
       </c>
-      <c r="C23">
-        <v>15</v>
-      </c>
-      <c r="D23">
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="E23">
-        <v>360</v>
-      </c>
-      <c r="F23">
-        <v>180</v>
-      </c>
-      <c r="H23">
+      <c r="E26">
+        <v>360</v>
+      </c>
+      <c r="F26">
+        <v>180</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="3"/>
         <v>2.4118095489747926</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
         <v>10</v>
       </c>
-      <c r="C24">
-        <v>15</v>
-      </c>
-      <c r="D24">
+      <c r="C27">
+        <v>15</v>
+      </c>
+      <c r="D27">
         <f t="shared" si="2"/>
         <v>135</v>
       </c>
-      <c r="E24">
-        <v>360</v>
-      </c>
-      <c r="F24">
+      <c r="E27">
+        <v>360</v>
+      </c>
+      <c r="F27">
         <v>225</v>
       </c>
-      <c r="H24">
+      <c r="H27">
         <f t="shared" si="3"/>
         <v>3.6602540378443864</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
         <v>10</v>
       </c>
-      <c r="C25">
-        <v>15</v>
-      </c>
-      <c r="D25">
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="E25">
-        <v>360</v>
-      </c>
-      <c r="F25">
+      <c r="E28">
+        <v>360</v>
+      </c>
+      <c r="F28">
         <v>270</v>
       </c>
-      <c r="H25">
+      <c r="H28">
         <f t="shared" si="3"/>
         <v>5.6301625030524702</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="B26">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
         <v>10</v>
       </c>
-      <c r="C26">
-        <v>15</v>
-      </c>
-      <c r="D26">
+      <c r="C29">
+        <v>15</v>
+      </c>
+      <c r="D29">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="E26">
-        <v>360</v>
-      </c>
-      <c r="F26">
+      <c r="E29">
+        <v>360</v>
+      </c>
+      <c r="F29">
         <v>315</v>
       </c>
-      <c r="H26">
+      <c r="H29">
         <f t="shared" si="3"/>
         <v>7.0710678118654746</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
         <v>10</v>
       </c>
-      <c r="C27">
-        <v>15</v>
-      </c>
-      <c r="D27">
+      <c r="C30">
+        <v>15</v>
+      </c>
+      <c r="D30">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E27">
-        <v>360</v>
-      </c>
-      <c r="F27">
-        <v>360</v>
-      </c>
-      <c r="H27">
+      <c r="E30">
+        <v>360</v>
+      </c>
+      <c r="F30">
+        <v>360</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="3"/>
         <v>7.5881904510252074</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>5</v>
-      </c>
-      <c r="B29">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
         <v>2.5</v>
       </c>
-      <c r="C29">
-        <v>15</v>
-      </c>
-      <c r="D29">
-        <f>+E29-F29</f>
-        <v>360</v>
-      </c>
-      <c r="E29">
-        <v>360</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <f>+B29*(((A29/B29)^2+2*(A29/B29)*SIN(C29/180*PI())*COS(D29/180*PI())+(SIN(C29/180*PI())^2))^0.5)</f>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <f>+E32-F32</f>
+        <v>360</v>
+      </c>
+      <c r="E32">
+        <v>360</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f>+B32*(((A32/B32)^2+2*(A32/B32)*SIN(C32/180*PI())*COS(D32/180*PI())+(SIN(C32/180*PI())^2))^0.5)</f>
         <v>5.6470476127563014</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>5</v>
-      </c>
-      <c r="B30">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
         <v>2.5</v>
       </c>
-      <c r="C30">
-        <v>15</v>
-      </c>
-      <c r="D30">
-        <f t="shared" ref="D30:D37" si="4">+E30-F30</f>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ref="D33:D40" si="4">+E33-F33</f>
         <v>315</v>
       </c>
-      <c r="E30">
-        <v>360</v>
-      </c>
-      <c r="F30">
+      <c r="E33">
+        <v>360</v>
+      </c>
+      <c r="F33">
         <v>45</v>
       </c>
-      <c r="H30">
-        <f t="shared" ref="H30:H37" si="5">+B30*(((A30/B30)^2+2*(A30/B30)*SIN(C30/180*PI())*COS(D30/180*PI())+(SIN(C30/180*PI())^2))^0.5)</f>
+      <c r="H33">
+        <f t="shared" ref="H33:H40" si="5">+B33*(((A33/B33)^2+2*(A33/B33)*SIN(C33/180*PI())*COS(D33/180*PI())+(SIN(C33/180*PI())^2))^0.5)</f>
         <v>5.4766767442016429</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>5</v>
-      </c>
-      <c r="B31">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
         <v>2.5</v>
       </c>
-      <c r="C31">
-        <v>15</v>
-      </c>
-      <c r="D31">
+      <c r="C34">
+        <v>15</v>
+      </c>
+      <c r="D34">
         <f t="shared" si="4"/>
         <v>270</v>
       </c>
-      <c r="E31">
-        <v>360</v>
-      </c>
-      <c r="F31">
+      <c r="E34">
+        <v>360</v>
+      </c>
+      <c r="F34">
         <v>90</v>
       </c>
-      <c r="H31">
+      <c r="H34">
         <f t="shared" si="5"/>
         <v>5.0416932287847143</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>5</v>
-      </c>
-      <c r="B32">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
         <v>2.5</v>
       </c>
-      <c r="C32">
-        <v>15</v>
-      </c>
-      <c r="D32">
+      <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="D35">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="E32">
-        <v>360</v>
-      </c>
-      <c r="F32">
+      <c r="E35">
+        <v>360</v>
+      </c>
+      <c r="F35">
         <v>135</v>
       </c>
-      <c r="H32">
+      <c r="H35">
         <f t="shared" si="5"/>
         <v>4.5654521206413001</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>5</v>
-      </c>
-      <c r="B33">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
         <v>2.5</v>
       </c>
-      <c r="C33">
-        <v>15</v>
-      </c>
-      <c r="D33">
+      <c r="C36">
+        <v>15</v>
+      </c>
+      <c r="D36">
         <f t="shared" si="4"/>
         <v>180</v>
       </c>
-      <c r="E33">
-        <v>360</v>
-      </c>
-      <c r="F33">
-        <v>180</v>
-      </c>
-      <c r="H33">
+      <c r="E36">
+        <v>360</v>
+      </c>
+      <c r="F36">
+        <v>180</v>
+      </c>
+      <c r="H36">
         <f t="shared" si="5"/>
         <v>4.3529523872436986</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>5</v>
-      </c>
-      <c r="B34">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
         <v>2.5</v>
       </c>
-      <c r="C34">
-        <v>15</v>
-      </c>
-      <c r="D34">
+      <c r="C37">
+        <v>15</v>
+      </c>
+      <c r="D37">
         <f t="shared" si="4"/>
         <v>135</v>
       </c>
-      <c r="E34">
-        <v>360</v>
-      </c>
-      <c r="F34">
+      <c r="E37">
+        <v>360</v>
+      </c>
+      <c r="F37">
         <v>225</v>
       </c>
-      <c r="H34">
+      <c r="H37">
         <f t="shared" si="5"/>
         <v>4.565452120641301</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>5</v>
-      </c>
-      <c r="B35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
         <v>2.5</v>
       </c>
-      <c r="C35">
-        <v>15</v>
-      </c>
-      <c r="D35">
+      <c r="C38">
+        <v>15</v>
+      </c>
+      <c r="D38">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="E35">
-        <v>360</v>
-      </c>
-      <c r="F35">
+      <c r="E38">
+        <v>360</v>
+      </c>
+      <c r="F38">
         <v>270</v>
       </c>
-      <c r="H35">
+      <c r="H38">
         <f t="shared" si="5"/>
         <v>5.0416932287847143</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J38" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>5</v>
-      </c>
-      <c r="B36">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
         <v>2.5</v>
       </c>
-      <c r="C36">
-        <v>15</v>
-      </c>
-      <c r="D36">
+      <c r="C39">
+        <v>15</v>
+      </c>
+      <c r="D39">
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="E36">
-        <v>360</v>
-      </c>
-      <c r="F36">
+      <c r="E39">
+        <v>360</v>
+      </c>
+      <c r="F39">
         <v>315</v>
       </c>
-      <c r="H36">
+      <c r="H39">
         <f t="shared" si="5"/>
         <v>5.4766767442016429</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>5</v>
-      </c>
-      <c r="B37">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
         <v>2.5</v>
       </c>
-      <c r="C37">
-        <v>15</v>
-      </c>
-      <c r="D37">
+      <c r="C40">
+        <v>15</v>
+      </c>
+      <c r="D40">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E37">
-        <v>360</v>
-      </c>
-      <c r="F37">
-        <v>360</v>
-      </c>
-      <c r="H37">
+      <c r="E40">
+        <v>360</v>
+      </c>
+      <c r="F40">
+        <v>360</v>
+      </c>
+      <c r="H40">
         <f t="shared" si="5"/>
         <v>5.6470476127563014</v>
       </c>
-      <c r="J37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>5</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <f>+E40-F40</f>
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <f>+B40*(((A40/B40)^2+2*(A40/B40)*SIN(C40/180*PI())*COS(D40/180*PI())+(SIN(C40/180*PI())^2))^0.5)</f>
-        <v>5</v>
-      </c>
       <c r="J40" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>5</v>
-      </c>
-      <c r="B41">
-        <v>5</v>
-      </c>
-      <c r="C41">
-        <v>5</v>
-      </c>
-      <c r="D41">
-        <f t="shared" ref="D41:D48" si="6">+E41-F41</f>
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <f>+B41*(((A41/B41)^2+2*(A41/B41)*SIN(C41/180*PI())*COS(D41/180*PI())+(SIN(C41/180*PI())^2))^0.5)</f>
-        <v>5.4357787137382907</v>
-      </c>
-      <c r="J41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>5</v>
-      </c>
-      <c r="B42">
-        <v>5</v>
-      </c>
-      <c r="C42">
-        <v>10</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <f>+B42*(((A42/B42)^2+2*(A42/B42)*SIN(C42/180*PI())*COS(D42/180*PI())+(SIN(C42/180*PI())^2))^0.5)</f>
-        <v>5.8682408883346513</v>
-      </c>
-      <c r="J42" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>5</v>
@@ -1299,10 +1240,10 @@
         <v>5</v>
       </c>
       <c r="C43">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <f t="shared" si="6"/>
+        <f>+E43-F43</f>
         <v>0</v>
       </c>
       <c r="E43">
@@ -1312,8 +1253,8 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <f>+B43*(((A43/B43)^2+2*(A43/B43)*SIN(C43/180*PI())*COS(D43/180*PI())+(SIN(C43/180*PI())^2))^0.5)</f>
-        <v>6.2940952255126037</v>
+        <f t="shared" ref="H43:H51" si="6">+B43*(((A43/B43)^2+2*(A43/B43)*SIN(C43/180*PI())*COS(D43/180*PI())+(SIN(C43/180*PI())^2))^0.5)</f>
+        <v>5</v>
       </c>
       <c r="J43" t="s">
         <v>17</v>
@@ -1327,21 +1268,21 @@
         <v>5</v>
       </c>
       <c r="C44">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D44">
+        <f t="shared" ref="D44:D51" si="7">+E44-F44</f>
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <f>+B44*(((A44/B44)^2+2*(A44/B44)*SIN(C44/180*PI())*COS(D44/180*PI())+(SIN(C44/180*PI())^2))^0.5)</f>
-        <v>6.7101007166283431</v>
+        <v>5.4357787137382907</v>
       </c>
       <c r="J44" t="s">
         <v>17</v>
@@ -1355,21 +1296,21 @@
         <v>5</v>
       </c>
       <c r="C45">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D45">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="H45">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <f>+B45*(((A45/B45)^2+2*(A45/B45)*SIN(C45/180*PI())*COS(D45/180*PI())+(SIN(C45/180*PI())^2))^0.5)</f>
-        <v>7.1130913087034973</v>
+        <v>5.8682408883346513</v>
       </c>
       <c r="J45" t="s">
         <v>17</v>
@@ -1383,21 +1324,21 @@
         <v>5</v>
       </c>
       <c r="C46">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D46">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="H46">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <f>+B46*(((A46/B46)^2+2*(A46/B46)*SIN(C46/180*PI())*COS(D46/180*PI())+(SIN(C46/180*PI())^2))^0.5)</f>
-        <v>7.5</v>
+        <v>6.2940952255126037</v>
       </c>
       <c r="J46" t="s">
         <v>17</v>
@@ -1411,21 +1352,21 @@
         <v>5</v>
       </c>
       <c r="C47">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D47">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="H47">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <f>+B47*(((A47/B47)^2+2*(A47/B47)*SIN(C47/180*PI())*COS(D47/180*PI())+(SIN(C47/180*PI())^2))^0.5)</f>
-        <v>7.8678821817552302</v>
+        <v>6.7101007166283431</v>
       </c>
       <c r="J47" t="s">
         <v>17</v>
@@ -1439,26 +1380,54 @@
         <v>5</v>
       </c>
       <c r="C48">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="H48">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <f>+B48*(((A48/B48)^2+2*(A48/B48)*SIN(C48/180*PI())*COS(D48/180*PI())+(SIN(C48/180*PI())^2))^0.5)</f>
-        <v>8.2139380484326967</v>
+        <v>7.1130913087034973</v>
       </c>
       <c r="J48" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>30</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+      <c r="J49" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5</v>
@@ -1467,24 +1436,24 @@
         <v>5</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D50">
-        <f>+E50-F50</f>
-        <v>180</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <f t="shared" ref="H50:H58" si="7">+B50*(((A50/B50)^2+2*(A50/B50)*SIN(C50/180*PI())*COS(D50/180*PI())+(SIN(C50/180*PI())^2))^0.5)</f>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>7.8678821817552302</v>
       </c>
       <c r="J50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -1495,52 +1464,24 @@
         <v>5</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D51">
-        <f t="shared" ref="D51:D58" si="8">+E51-F51</f>
-        <v>180</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H51">
-        <f t="shared" si="7"/>
-        <v>4.5642212862617093</v>
+        <f t="shared" si="6"/>
+        <v>8.2139380484326967</v>
       </c>
       <c r="J51" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>5</v>
-      </c>
-      <c r="B52">
-        <v>5</v>
-      </c>
-      <c r="C52">
-        <v>10</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="8"/>
-        <v>180</v>
-      </c>
-      <c r="E52">
-        <v>360</v>
-      </c>
-      <c r="F52">
-        <v>180</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="7"/>
-        <v>4.1317591116653487</v>
-      </c>
-      <c r="J52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -1551,10 +1492,10 @@
         <v>5</v>
       </c>
       <c r="C53">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <f t="shared" si="8"/>
+        <f>+E53-F53</f>
         <v>180</v>
       </c>
       <c r="E53">
@@ -1564,8 +1505,8 @@
         <v>180</v>
       </c>
       <c r="H53">
-        <f t="shared" si="7"/>
-        <v>3.7059047744873963</v>
+        <f t="shared" ref="H53:H61" si="8">+B53*(((A53/B53)^2+2*(A53/B53)*SIN(C53/180*PI())*COS(D53/180*PI())+(SIN(C53/180*PI())^2))^0.5)</f>
+        <v>5</v>
       </c>
       <c r="J53" t="s">
         <v>18</v>
@@ -1579,21 +1520,21 @@
         <v>5</v>
       </c>
       <c r="C54">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D54">
+        <f t="shared" ref="D54:D61" si="9">+E54-F54</f>
+        <v>180</v>
+      </c>
+      <c r="E54">
+        <v>360</v>
+      </c>
+      <c r="F54">
+        <v>180</v>
+      </c>
+      <c r="H54">
         <f t="shared" si="8"/>
-        <v>180</v>
-      </c>
-      <c r="E54">
-        <v>360</v>
-      </c>
-      <c r="F54">
-        <v>180</v>
-      </c>
-      <c r="H54">
-        <f t="shared" si="7"/>
-        <v>3.289899283371656</v>
+        <v>4.5642212862617093</v>
       </c>
       <c r="J54" t="s">
         <v>18</v>
@@ -1607,21 +1548,21 @@
         <v>5</v>
       </c>
       <c r="C55">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D55">
+        <f t="shared" si="9"/>
+        <v>180</v>
+      </c>
+      <c r="E55">
+        <v>360</v>
+      </c>
+      <c r="F55">
+        <v>180</v>
+      </c>
+      <c r="H55">
         <f t="shared" si="8"/>
-        <v>180</v>
-      </c>
-      <c r="E55">
-        <v>360</v>
-      </c>
-      <c r="F55">
-        <v>180</v>
-      </c>
-      <c r="H55">
-        <f t="shared" si="7"/>
-        <v>2.8869086912965032</v>
+        <v>4.1317591116653487</v>
       </c>
       <c r="J55" t="s">
         <v>18</v>
@@ -1635,21 +1576,21 @@
         <v>5</v>
       </c>
       <c r="C56">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D56">
+        <f t="shared" si="9"/>
+        <v>180</v>
+      </c>
+      <c r="E56">
+        <v>360</v>
+      </c>
+      <c r="F56">
+        <v>180</v>
+      </c>
+      <c r="H56">
         <f t="shared" si="8"/>
-        <v>180</v>
-      </c>
-      <c r="E56">
-        <v>360</v>
-      </c>
-      <c r="F56">
-        <v>180</v>
-      </c>
-      <c r="H56">
-        <f t="shared" si="7"/>
-        <v>2.5</v>
+        <v>3.7059047744873963</v>
       </c>
       <c r="J56" t="s">
         <v>18</v>
@@ -1663,21 +1604,21 @@
         <v>5</v>
       </c>
       <c r="C57">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D57">
+        <f t="shared" si="9"/>
+        <v>180</v>
+      </c>
+      <c r="E57">
+        <v>360</v>
+      </c>
+      <c r="F57">
+        <v>180</v>
+      </c>
+      <c r="H57">
         <f t="shared" si="8"/>
-        <v>180</v>
-      </c>
-      <c r="E57">
-        <v>360</v>
-      </c>
-      <c r="F57">
-        <v>180</v>
-      </c>
-      <c r="H57">
-        <f t="shared" si="7"/>
-        <v>2.1321178182447698</v>
+        <v>3.289899283371656</v>
       </c>
       <c r="J57" t="s">
         <v>18</v>
@@ -1691,23 +1632,107 @@
         <v>5</v>
       </c>
       <c r="C58">
+        <v>25</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="9"/>
+        <v>180</v>
+      </c>
+      <c r="E58">
+        <v>360</v>
+      </c>
+      <c r="F58">
+        <v>180</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="8"/>
+        <v>2.8869086912965032</v>
+      </c>
+      <c r="J58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>30</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="9"/>
+        <v>180</v>
+      </c>
+      <c r="E59">
+        <v>360</v>
+      </c>
+      <c r="F59">
+        <v>180</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="J59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <v>35</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="9"/>
+        <v>180</v>
+      </c>
+      <c r="E60">
+        <v>360</v>
+      </c>
+      <c r="F60">
+        <v>180</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="8"/>
+        <v>2.1321178182447698</v>
+      </c>
+      <c r="J60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
         <v>40</v>
       </c>
-      <c r="D58">
+      <c r="D61">
+        <f t="shared" si="9"/>
+        <v>180</v>
+      </c>
+      <c r="E61">
+        <v>360</v>
+      </c>
+      <c r="F61">
+        <v>180</v>
+      </c>
+      <c r="H61">
         <f t="shared" si="8"/>
-        <v>180</v>
-      </c>
-      <c r="E58">
-        <v>360</v>
-      </c>
-      <c r="F58">
-        <v>180</v>
-      </c>
-      <c r="H58">
-        <f t="shared" si="7"/>
         <v>1.7860619515673037</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J61" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>